<commit_message>
feat: Enhance import functionality to support additional fields for companies, registrations, and contacts, including DUNS number, social media URLs, and established date
</commit_message>
<xml_diff>
--- a/apps/web/lib/template/selly-base-template.xlsx
+++ b/apps/web/lib/template/selly-base-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6FE432-1813-4F14-A06A-9A32ACA16EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918C9925-1797-47A4-9111-3359CD353118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,93 +15,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Name (TH)</t>
-  </si>
-  <si>
-    <t>Local Name</t>
-  </si>
-  <si>
-    <t>Registration No</t>
-  </si>
-  <si>
-    <t>Registration Country</t>
-  </si>
-  <si>
-    <t>DUNS Number</t>
-  </si>
-  <si>
-    <t>Address Line 1</t>
-  </si>
-  <si>
-    <t>Address Line 2</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>Business Description</t>
-  </si>
-  <si>
-    <t>Established Date</t>
-  </si>
-  <si>
-    <t>Employee Count Estimate</t>
-  </si>
-  <si>
-    <t>Company Size</t>
-  </si>
-  <si>
-    <t>Annual Revenue Estimate</t>
-  </si>
-  <si>
-    <t>Currency Code</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>LinkedIn URL</t>
-  </si>
-  <si>
-    <t>Facebook URL</t>
-  </si>
-  <si>
-    <t>Primary Email</t>
-  </si>
-  <si>
-    <t>Primary Phone</t>
-  </si>
-  <si>
-    <t>Logo URL</t>
-  </si>
-  <si>
-    <t>Primary Industry</t>
-  </si>
-  <si>
-    <t>Primary Region</t>
-  </si>
-  <si>
-    <t>Contact Phones</t>
-  </si>
-  <si>
-    <t>Contact Emails</t>
-  </si>
-  <si>
-    <t>Data Quality Score</t>
-  </si>
-  <si>
-    <t>Data Sensitivity</t>
-  </si>
-  <si>
-    <t>Verification Status</t>
-  </si>
-  <si>
-    <t>Last Enriched At</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>duns_number</t>
+  </si>
+  <si>
+    <t>address_line_1</t>
+  </si>
+  <si>
+    <t>address_line_2</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>business_description</t>
+  </si>
+  <si>
+    <t>established_date</t>
+  </si>
+  <si>
+    <t>employee_count_estimate</t>
+  </si>
+  <si>
+    <t>website_url</t>
+  </si>
+  <si>
+    <t>facebook_url</t>
+  </si>
+  <si>
+    <t>registration_no</t>
+  </si>
+  <si>
+    <t>registration_type</t>
+  </si>
+  <si>
+    <t>registered_date</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>company_nameEn</t>
+  </si>
+  <si>
+    <t>company_nameTh</t>
+  </si>
+  <si>
+    <t>company_email</t>
+  </si>
+  <si>
+    <t>company_phone</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>authority</t>
+  </si>
+  <si>
+    <t>contact_email</t>
+  </si>
+  <si>
+    <t>contact_phone</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
@@ -111,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +114,14 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,10 +141,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -155,17 +155,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,40 +506,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -544,95 +546,91 @@
   <sheetData>
     <row r="1" spans="1:29" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="R1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="V1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="AC1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L2" s="8"/>
+      <c r="Y2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>